<commit_message>
Update schema if method name is changed in code pane.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Finish Save Project</t>
-  </si>
-  <si>
-    <t>Make sure to call code updateMethod if method name is changed either in edit method dialog or Blockly name change.</t>
   </si>
   <si>
     <t>Only use is in Type.js#m_functionUpdateActiveMethodWorkspace.</t>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>Occasionally, opening a project can take 2 minutes.</t>
+  </si>
+  <si>
+    <t>Make sure to call code.js#replaceMethod if method name is changed in Blockly name change.</t>
+  </si>
+  <si>
+    <t>It looks like it's hung on the client side retrieving the first image for the left vertical scroll pane.</t>
   </si>
 </sst>
 </file>
@@ -524,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -544,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -558,57 +561,57 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="3" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -616,117 +619,120 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="22" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
If they delete the function block, I reload from method.workspace.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -126,9 +126,6 @@
     <t>TO DO (Other)</t>
   </si>
   <si>
-    <t>As soon as we convert the workspace XML to JSON, we do have an array of &lt;block&gt; nodes. We can fairly easily recognize function blocks (there may be none or one or more) and other blocks (called 'chaff').</t>
-  </si>
-  <si>
     <t>See note and code in Code.js#self.blocklyChangeListener.</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>It looks like it's hung on the client side retrieving the first image for the left vertical scroll pane.</t>
+  </si>
+  <si>
+    <t>As soon as we convert the workspace XML to JSON, we do have an array of &lt;block&gt; nodes. We can fairly easily recognize function blocks (there may be none or one or more) and other blocks (called 'chaff'). Note: the solution does lose any chaff.</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,35 +641,35 @@
     </row>
     <row r="16" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>30</v>
@@ -683,23 +683,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
+    <row r="22" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
@@ -729,10 +729,10 @@
     </row>
     <row r="33" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Good work done in block manipulation.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>May be done. Needs testing.</t>
+  </si>
+  <si>
+    <t>Need to refresh TW header when method name changes.</t>
+  </si>
+  <si>
+    <t>Saving project is quite messed up.</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,58 +712,69 @@
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
+    <row r="24" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected a null instead of 10000 for ordinal of system base type. Pushing to have a revert point.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -546,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,14 +780,15 @@
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I do believe Saving Project works.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -156,25 +156,19 @@
     <t>Retain chaff when user deletes the only function c-block or we otherwise fall thru the worpaceJSON.children loop.</t>
   </si>
   <si>
-    <t>Methods (and probably more) are no longer being written to the database for a new project.</t>
-  </si>
-  <si>
-    <t>ordinal isn't being incremented for subsequent types in a comic when writing to the database for a new project.</t>
-  </si>
-  <si>
     <t>May be done. Needs testing.</t>
   </si>
   <si>
     <t>Need to refresh TW header when method name changes.</t>
   </si>
   <si>
-    <t>Saving project is quite messed up.</t>
-  </si>
-  <si>
     <t>Had to comment out Type.js line 296 (call to code.replaceMethod). It forces 2 passes thru BlocklyChangeListener and removes focus from name change after each character is typed.</t>
   </si>
   <si>
     <t>Discuss w/Ken.</t>
+  </si>
+  <si>
+    <t>Saving project is a little messed up.</t>
   </si>
 </sst>
 </file>
@@ -549,7 +543,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,73 +717,63 @@
         <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="4" t="s">
+    </row>
+    <row r="27" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
+    <row r="34" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now load all system base types with every project. Any new type can inherit from any system base type EXCEPT this project's SBT.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -120,12 +120,6 @@
     <t>It may already be being done in the dialog.</t>
   </si>
   <si>
-    <t>TO DO (Blockly-related)</t>
-  </si>
-  <si>
-    <t>TO DO (Other)</t>
-  </si>
-  <si>
     <t>See note and code in Code.js#self.blocklyChangeListener.</t>
   </si>
   <si>
@@ -169,6 +163,33 @@
   </si>
   <si>
     <t>Saving project is a little messed up.</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>Save project is still broken.</t>
+  </si>
+  <si>
+    <t>Load all system base types with every project.</t>
+  </si>
+  <si>
+    <t>Kill the system base type table.</t>
+  </si>
+  <si>
+    <t>Set up the droplist for new classes' base type choice to include all types EXCEPT the App type in this comic and the 1 base type that that App type is derived from. All other system base types should be included.</t>
+  </si>
+  <si>
+    <t>Double res.json({});</t>
+  </si>
+  <si>
+    <t>Save system base types when the project is saved, updating their former record so that their id stays the same. But deleting and then inserting of methods, props and events is the way to go for them.</t>
+  </si>
+  <si>
+    <t>See if I can auto-update the system base type SQL script when a project with system base types maintenance is saved.</t>
+  </si>
+  <si>
+    <t>Or always, if I don't know.</t>
   </si>
 </sst>
 </file>
@@ -540,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,35 +677,35 @@
     </row>
     <row r="16" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>30</v>
@@ -703,77 +724,107 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Progressing toward save new and edited SBTs with Project Save and SaveAs. SS
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Or always, if I don't know.</t>
+  </si>
+  <si>
+    <t>Delete current type should be disabled for: App Type; any SBT; any Type in the current Comic that is a base type for another type in that comic.</t>
+  </si>
+  <si>
+    <t>A New SBT should require an image.</t>
+  </si>
+  <si>
+    <t>Think more about deleting SBTs beyond the first 5.</t>
   </si>
 </sst>
 </file>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,42 +785,42 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
+    <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" s="3" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -825,6 +834,19 @@
       </c>
       <c r="B38" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project save is still not tested, but I did add checkbox in new project dialog to turn on editing SBTs.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Keep the chaff.</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Think more about deleting SBTs beyond the first 5.</t>
+  </si>
+  <si>
+    <t>Don't forget to delete m, p, e from updated SBTs.</t>
+  </si>
+  <si>
+    <t>Why did it work?</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,6 +855,16 @@
         <v>56</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
I don't let them delete a non-SBT base type if some other type points to it. Also fixed my neg id increment for new types.
</commit_message>
<xml_diff>
--- a/current work.xlsx
+++ b/current work.xlsx
@@ -597,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,9 +846,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+    <row r="36" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
@@ -913,13 +914,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>